<commit_message>
Finish Downloading Data from API
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\chame\Documents\UiPath\KRS_Data_Scraper\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{127947CB-7D8B-4121-BEF1-9054F58978FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7532E234-1DE4-44D3-B877-BE2EA3B2DF42}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2295" yWindow="2295" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="51">
   <si>
     <t>Name</t>
   </si>
@@ -166,6 +166,18 @@
   </si>
   <si>
     <t>Data\Input\Input.xlsx</t>
+  </si>
+  <si>
+    <t>KRSFinalExcelFilePath</t>
+  </si>
+  <si>
+    <t>Data\Output\Output_data.xlsx</t>
+  </si>
+  <si>
+    <t>KRSBaseRequestUrl</t>
+  </si>
+  <si>
+    <t>https://api-krs.ms.gov.pl/api/krs/OdpisAktualny/{krs}?rejestr=P&amp;format=json</t>
   </si>
 </sst>
 </file>
@@ -217,7 +229,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -227,6 +239,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normalny" xfId="0" builtinId="0"/>
@@ -544,13 +557,13 @@
   <dimension ref="A1:Z998"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="43.5703125" customWidth="1"/>
-    <col min="2" max="2" width="43" customWidth="1"/>
+    <col min="2" max="2" width="74.140625" customWidth="1"/>
     <col min="3" max="3" width="81.42578125" customWidth="1"/>
     <col min="4" max="26" width="8.7109375" customWidth="1"/>
   </cols>
@@ -630,9 +643,23 @@
         <v>46</v>
       </c>
     </row>
-    <row r="8" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="8" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A8" t="s">
+        <v>47</v>
+      </c>
+      <c r="B8" t="s">
+        <v>48</v>
+      </c>
+    </row>
     <row r="9" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="10" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="10" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A10" t="s">
+        <v>49</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>50</v>
+      </c>
+    </row>
     <row r="11" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="12" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="13" spans="1:26" ht="14.25" customHeight="1"/>
@@ -1633,7 +1660,7 @@
   <dimension ref="A1:Z988"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -1683,7 +1710,7 @@
         <v>5</v>
       </c>
       <c r="B2">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>25</v>
@@ -1694,7 +1721,7 @@
         <v>33</v>
       </c>
       <c r="B3">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>41</v>
@@ -1808,7 +1835,7 @@
         <v>40</v>
       </c>
       <c r="B17" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C17" s="3" t="s">
         <v>42</v>

</xml_diff>